<commit_message>
Replace repository with new v1.0.0 codebase
This commit replaces all old alpha-version code with the finalized and fully functional SOMBA framework for the v1.0.0 release associated with the publication in ES&T.
</commit_message>
<xml_diff>
--- a/SOMBA_template.xlsx
+++ b/SOMBA_template.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ts2264/Documents/Yale/papers/in_progress/in_prep/2024_Suhrhoff_JLM/soil_analysis/paper/SOMBA_user_example/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ts2264/Documents/publications/1_in_progress/2_submitted/2024_Suhrhoff_JLM/soil_analysis/method_paper/SOMBA_user_example/final publication/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47A8A8A5-9495-984E-8A2D-D6B9867BC1D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80FD5115-66D1-8742-94F7-723D0DCBA316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{29FD1345-78A7-A04A-B76B-806025C21648}"/>
+    <workbookView xWindow="920" yWindow="5900" windowWidth="26040" windowHeight="14940" xr2:uid="{6F829724-E138-2047-8EBF-A1702B6D4883}"/>
   </bookViews>
   <sheets>
-    <sheet name="example_data" sheetId="1" r:id="rId1"/>
+    <sheet name="model_verification_data_non_sim" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>site</t>
   </si>
@@ -41,10 +41,31 @@
     <t>[j]_s [mol/kg]</t>
   </si>
   <si>
+    <t>[i]_s [mol/kg]</t>
+  </si>
+  <si>
     <t>[j]_f [mol/kg]</t>
   </si>
   <si>
-    <t>[i]_s [mol/kg]</t>
+    <t>[i]_f [mol/kg]</t>
+  </si>
+  <si>
+    <t>[j]_wf [mol/kg]</t>
+  </si>
+  <si>
+    <t>[i]_wf [mol/kg]</t>
+  </si>
+  <si>
+    <t>ρ_s [t/m3]</t>
+  </si>
+  <si>
+    <t>ρ_f [t/m3]</t>
+  </si>
+  <si>
+    <t>ρ_wf [t/m3]</t>
+  </si>
+  <si>
+    <t>v_sampled_layer [m3/ha]</t>
   </si>
   <si>
     <t>[j]_mix,t=n [mol/kg]</t>
@@ -53,64 +74,31 @@
     <t>[i]_mix,t=n [mol/kg]</t>
   </si>
   <si>
-    <t>ρ_s [t/m3]</t>
-  </si>
-  <si>
-    <t>ρ_f [t/m3]</t>
-  </si>
-  <si>
-    <t>v_sampled_layer [m3/ha]</t>
-  </si>
-  <si>
-    <t>[i]_f [mol/kg]</t>
-  </si>
-  <si>
-    <t>a (eq. S13a)</t>
-  </si>
-  <si>
-    <t>b (eq. S13b)</t>
-  </si>
-  <si>
-    <t>c (eq. S13c)</t>
-  </si>
-  <si>
-    <t>d (eq. S13d)</t>
-  </si>
-  <si>
-    <t>e (eq. S13e)</t>
-  </si>
-  <si>
-    <t>X_f [] (eq. 6)</t>
-  </si>
-  <si>
-    <t>X_wf [] (eq. 7)</t>
-  </si>
-  <si>
-    <t>X_s [] (eq. 8)</t>
-  </si>
-  <si>
-    <t>τ_j [] (eq. 9)</t>
-  </si>
-  <si>
-    <t>a [t/ha] (eq. 10)</t>
-  </si>
-  <si>
-    <t>[j]_mix,t=0 [mol/kg] (eq. 11)</t>
-  </si>
-  <si>
-    <t>[i]_mix,t=0 [mol/kg] (eq. 12)</t>
-  </si>
-  <si>
-    <t>[i]_wf [mol/kg] (eq.S1)</t>
+    <t>τ_j []</t>
+  </si>
+  <si>
+    <t>X_s []</t>
+  </si>
+  <si>
+    <t>X_f []</t>
+  </si>
+  <si>
+    <t>X_wf []</t>
+  </si>
+  <si>
+    <t>a [t/ha]</t>
+  </si>
+  <si>
+    <t>[j]_(mix,t=0)</t>
+  </si>
+  <si>
+    <t>[i]_(mix,t=0)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.000"/>
-  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -588,10 +576,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -966,33 +953,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD2AAAF9-0CFD-BC49-88B6-1D5275BD17D6}">
-  <dimension ref="A1:W11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15506C41-500D-8848-B503-E9B9E7E47384}">
+  <dimension ref="A1:T11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="25.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.33203125" customWidth="1"/>
-    <col min="19" max="19" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="23" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" customWidth="1"/>
+    <col min="11" max="11" width="20" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="11" customWidth="1"/>
+    <col min="16" max="16" width="11.5" customWidth="1"/>
+    <col min="17" max="17" width="11" customWidth="1"/>
+    <col min="18" max="18" width="12.6640625" customWidth="1"/>
+    <col min="19" max="19" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1000,28 +981,28 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>9</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" t="s">
         <v>10</v>
@@ -1033,16 +1014,16 @@
         <v>12</v>
       </c>
       <c r="N1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" t="s">
+        <v>16</v>
+      </c>
+      <c r="P1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" t="s">
         <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
       </c>
       <c r="R1" t="s">
         <v>17</v>
@@ -1053,854 +1034,695 @@
       <c r="T1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" t="s">
-        <v>22</v>
-      </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>0.52691933563511795</v>
+        <v>0.48618346907481702</v>
       </c>
       <c r="C2" s="1">
-        <v>4.2106545325074096</v>
+        <v>3.7669152429692501</v>
       </c>
       <c r="D2" s="1">
-        <v>5.2523368944178403E-2</v>
+        <v>0.57073864572700606</v>
       </c>
       <c r="E2" s="1">
-        <v>0.23824493930822599</v>
+        <v>5.0207906927160199E-2</v>
       </c>
       <c r="F2" s="1">
-        <v>0.643874189261466</v>
+        <v>0.23907997271063</v>
       </c>
       <c r="G2" s="1">
-        <v>6.8724901949025904E-2</v>
+        <v>0.35004113449007601</v>
       </c>
       <c r="H2" s="1">
-        <v>1.3827562484617699</v>
+        <v>1.4680688753126201</v>
       </c>
       <c r="I2" s="1">
-        <v>1.83164648189201</v>
+        <v>1.8411238054741099</v>
       </c>
       <c r="J2" s="1">
+        <v>1.54446021838951</v>
+      </c>
+      <c r="K2">
         <v>1000</v>
       </c>
-      <c r="K2" s="2">
-        <f>H2*(F2-B2)</f>
-        <v>0.16172005463976447</v>
-      </c>
       <c r="L2" s="1">
-        <f>I2*(F2-C2)</f>
-        <v>-6.5330806673880089</v>
+        <v>0.59420242860297101</v>
       </c>
       <c r="M2" s="1">
-        <f>H2*(G2-D2)</f>
-        <v>2.2402770997112478E-2</v>
+        <v>6.0531622379625602E-2</v>
       </c>
       <c r="N2" s="1">
-        <f>I2*(G2-E2)</f>
-        <v>-0.31050078003918091</v>
+        <f>(-(J2*(M2-G2)-(J2*(L2-D2)*H2*(M2-E2))/(H2*(L2-B2)))/(I2*(M2-F2)-(I2*(L2-C2)*H2*(M2-E2))/(H2*(L2-B2))))/((-(J2*(M2-G2)-(J2*(L2-D2)*H2*(M2-E2))/(H2*(L2-B2)))/(I2*(M2-F2)-(I2*(L2-C2)*H2*(M2-E2))/(H2*(L2-B2))))+((-I2*(L2-C2)*(-(J2*(M2-G2)-(J2*(L2-D2)*H2*(M2-E2))/(H2*(L2-B2)))/(I2*(M2-F2)-(I2*(L2-C2)*H2*(M2-E2))/(H2*(L2-B2))))-J2*(L2-D2))/(H2*(L2-B2)))+1)</f>
+        <v>2.6158441953871743E-2</v>
       </c>
       <c r="O2" s="1">
-        <f>I2*E2</f>
-        <v>0.43638050491248759</v>
+        <f>1/((-(J2*(M2-G2)-(J2*(L2-D2)*H2*(M2-E2))/(H2*(L2-B2)))/(I2*(M2-F2)-(I2*(L2-C2)*H2*(M2-E2))/(H2*(L2-B2))))+((-I2*(L2-C2)*(-(J2*(M2-G2)-(J2*(L2-D2)*H2*(M2-E2))/(H2*(L2-B2)))/(I2*(M2-F2)-(I2*(L2-C2)*H2*(M2-E2))/(H2*(L2-B2))))-J2*(L2-D2))/(H2*(L2-B2)))+1)</f>
+        <v>1.332581421963769E-2</v>
       </c>
       <c r="P2" s="1">
-        <f>K2/(K2-L2)</f>
-        <v>2.4156066977118543E-2</v>
+        <f>1-N2-O2</f>
+        <v>0.96051574382649052</v>
       </c>
       <c r="Q2" s="1">
-        <f>(K2*N2-L2*M2)/(O2*(K2-L2))</f>
-        <v>3.2909651920035199E-2</v>
+        <f t="shared" ref="Q2:Q11" si="0">O2/(O2+N2)</f>
+        <v>0.33749690410979999</v>
       </c>
       <c r="R2" s="1">
-        <f>1-P2-Q2</f>
-        <v>0.94293428110284627</v>
+        <f>(N2+O2)*K2*I2</f>
+        <v>72.695403982486297</v>
       </c>
       <c r="S2" s="1">
-        <f>Q2/(Q2+P2)</f>
-        <v>0.57669740355582599</v>
+        <f>(H2*P2*B2 + I2*(N2+O2)*C2) / (H2*P2 + I2*(N2+O2))</f>
+        <v>0.64702399733160687</v>
       </c>
       <c r="T2" s="1">
-        <f>(P2+Q2)*J2*I2</f>
-        <v>104.52422325461005</v>
-      </c>
-      <c r="U2" s="1">
-        <f>(H2*R2*B2+I2*(P2+Q2)*C2)/(H2*R2+I2*(P2+Q2))</f>
-        <v>0.80031260497499812</v>
-      </c>
-      <c r="V2" s="1">
-        <f>(H2*R2*D2+I2*(P2+Q2)*E2)/(H2*R2+I2*(P2+Q2))</f>
-        <v>6.6306940399551886E-2</v>
-      </c>
-      <c r="W2" s="1">
-        <f>D2+E2*I2/H2</f>
-        <v>0.36811080917302114</v>
+        <f>(H2*P2*E2 + I2*(N2+O2)*F2) / (H2*P2 + I2*(N2+O2))</f>
+        <v>5.9467512688073577E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>0.47268965405901298</v>
+        <v>0.50891246731247897</v>
       </c>
       <c r="C3" s="1">
-        <v>4.3294341352648198</v>
+        <v>3.93807928790017</v>
       </c>
       <c r="D3" s="1">
-        <v>5.2685161600259503E-2</v>
+        <v>0.52540156557461404</v>
       </c>
       <c r="E3" s="1">
-        <v>0.25510590754122398</v>
+        <v>4.6254607836893599E-2</v>
       </c>
       <c r="F3" s="1">
-        <v>0.69671526814162099</v>
+        <v>0.25172870864965402</v>
       </c>
       <c r="G3" s="1">
-        <v>7.0986292961542602E-2</v>
+        <v>0.40949399855847601</v>
       </c>
       <c r="H3" s="1">
-        <v>1.2831813078079599</v>
+        <v>1.3766129763824799</v>
       </c>
       <c r="I3" s="1">
-        <v>1.76366649842215</v>
+        <v>1.98642443876568</v>
       </c>
       <c r="J3" s="1">
+        <v>1.6123150778885</v>
+      </c>
+      <c r="K3">
         <v>1000</v>
       </c>
-      <c r="K3" s="2">
-        <f t="shared" ref="K3:K11" si="0">H3*(F3-B3)</f>
-        <v>0.28746548046100229</v>
-      </c>
       <c r="L3" s="1">
-        <f t="shared" ref="L3:L11" si="1">I3*(F3-C3)</f>
-        <v>-6.406904564131251</v>
+        <v>0.87857774384259202</v>
       </c>
       <c r="M3" s="1">
-        <f t="shared" ref="M3:M11" si="2">H3*(G3-D3)</f>
-        <v>2.3483669674536516E-2</v>
+        <v>8.3142591035309701E-2</v>
       </c>
       <c r="N3" s="1">
-        <f t="shared" ref="N3:N11" si="3">I3*(G3-E3)</f>
-        <v>-0.32472559593658246</v>
+        <f>(-(J3*(M3-G3)-(J3*(L3-D3)*H3*(M3-E3))/(H3*(L3-B3)))/(I3*(M3-F3)-(I3*(L3-C3)*H3*(M3-E3))/(H3*(L3-B3))))/((-(J3*(M3-G3)-(J3*(L3-D3)*H3*(M3-E3))/(H3*(L3-B3)))/(I3*(M3-F3)-(I3*(L3-C3)*H3*(M3-E3))/(H3*(L3-B3))))+((-I3*(L3-C3)*(-(J3*(M3-G3)-(J3*(L3-D3)*H3*(M3-E3))/(H3*(L3-B3)))/(I3*(M3-F3)-(I3*(L3-C3)*H3*(M3-E3))/(H3*(L3-B3))))-J3*(L3-D3))/(H3*(L3-B3)))+1)</f>
+        <v>7.7595950319576085E-2</v>
       </c>
       <c r="O3" s="1">
-        <f t="shared" ref="O3:O11" si="4">I3*E3</f>
-        <v>0.44992174268003521</v>
+        <f>1/((-(J3*(M3-G3)-(J3*(L3-D3)*H3*(M3-E3))/(H3*(L3-B3)))/(I3*(M3-F3)-(I3*(L3-C3)*H3*(M3-E3))/(H3*(L3-B3))))+((-I3*(L3-C3)*(-(J3*(M3-G3)-(J3*(L3-D3)*H3*(M3-E3))/(H3*(L3-B3)))/(I3*(M3-F3)-(I3*(L3-C3)*H3*(M3-E3))/(H3*(L3-B3))))-J3*(L3-D3))/(H3*(L3-B3)))+1)</f>
+        <v>3.614538797250981E-2</v>
       </c>
       <c r="P3" s="1">
-        <f t="shared" ref="P3:P11" si="5">K3/(K3-L3)</f>
-        <v>4.2941378881978354E-2</v>
+        <f t="shared" ref="P3:P11" si="1">1-N3-O3</f>
+        <v>0.88625866170791412</v>
       </c>
       <c r="Q3" s="1">
-        <f t="shared" ref="Q3:Q11" si="6">(K3*N3-L3*M3)/(O3*(K3-L3))</f>
-        <v>1.8961261171547682E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.31778585090751305</v>
       </c>
       <c r="R3" s="1">
-        <f t="shared" ref="R3:R11" si="7">1-P3-Q3</f>
-        <v>0.93809735994647392</v>
+        <f>(N3+O3)*K3*I3</f>
+        <v>225.93857408131407</v>
       </c>
       <c r="S3" s="1">
-        <f t="shared" ref="S3:S11" si="8">Q3/(Q3+P3)</f>
-        <v>0.30630779487195114</v>
+        <f>(H3*P3*B3 + I3*(N3+O3)*C3) / (H3*P3 + I3*(N3+O3))</f>
+        <v>1.0447320578717147</v>
       </c>
       <c r="T3" s="1">
-        <f t="shared" ref="T3:T11" si="9">(P3+Q3)*J3*I3</f>
-        <v>109.17561242628901</v>
-      </c>
-      <c r="U3" s="1">
-        <f t="shared" ref="U3:U11" si="10">(H3*R3*B3+I3*(P3+Q3)*C3)/(H3*R3+I3*(P3+Q3))</f>
-        <v>0.79339538051445269</v>
-      </c>
-      <c r="V3" s="1">
-        <f t="shared" ref="V3:V11" si="11">(H3*R3*D3+I3*(P3+Q3)*E3)/(H3*R3+I3*(P3+Q3))</f>
-        <v>6.951736106096959E-2</v>
-      </c>
-      <c r="W3" s="1">
-        <f t="shared" ref="W3:W11" si="12">D3+E3*I3/H3</f>
-        <v>0.4033150686463885</v>
+        <f>(H3*P3*E3 + I3*(N3+O3)*F3) / (H3*P3 + I3*(N3+O3))</f>
+        <v>7.8360671591806527E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>0.52730409879645301</v>
+        <v>0.49458522599883797</v>
       </c>
       <c r="C4" s="1">
-        <v>3.92247070352636</v>
+        <v>4.2239390188405102</v>
       </c>
       <c r="D4" s="1">
-        <v>5.0390404013412403E-2</v>
+        <v>0.55192640213873601</v>
       </c>
       <c r="E4" s="1">
-        <v>0.23484443469837399</v>
+        <v>5.1076944475075797E-2</v>
       </c>
       <c r="F4" s="1">
-        <v>0.56350409877716601</v>
+        <v>0.251267174813122</v>
       </c>
       <c r="G4" s="1">
-        <v>6.2178372862539702E-2</v>
+        <v>0.34085863837148</v>
       </c>
       <c r="H4" s="1">
-        <v>1.4797174282797301</v>
+        <v>1.4708593947149899</v>
       </c>
       <c r="I4" s="1">
-        <v>1.80555301793603</v>
+        <v>1.6963144000045201</v>
       </c>
       <c r="J4" s="1">
+        <v>1.62557479569442</v>
+      </c>
+      <c r="K4">
         <v>1000</v>
       </c>
-      <c r="K4" s="2">
+      <c r="L4" s="1">
+        <v>0.77353234173302898</v>
+      </c>
+      <c r="M4" s="1">
+        <v>7.1085443659790803E-2</v>
+      </c>
+      <c r="N4" s="1">
+        <f>(-(J4*(M4-G4)-(J4*(L4-D4)*H4*(M4-E4))/(H4*(L4-B4)))/(I4*(M4-F4)-(I4*(L4-C4)*H4*(M4-E4))/(H4*(L4-B4))))/((-(J4*(M4-G4)-(J4*(L4-D4)*H4*(M4-E4))/(H4*(L4-B4)))/(I4*(M4-F4)-(I4*(L4-C4)*H4*(M4-E4))/(H4*(L4-B4))))+((-I4*(L4-C4)*(-(J4*(M4-G4)-(J4*(L4-D4)*H4*(M4-E4))/(H4*(L4-B4)))/(I4*(M4-F4)-(I4*(L4-C4)*H4*(M4-E4))/(H4*(L4-B4))))-J4*(L4-D4))/(H4*(L4-B4)))+1)</f>
+        <v>6.5379195803590098E-2</v>
+      </c>
+      <c r="O4" s="1">
+        <f>1/((-(J4*(M4-G4)-(J4*(L4-D4)*H4*(M4-E4))/(H4*(L4-B4)))/(I4*(M4-F4)-(I4*(L4-C4)*H4*(M4-E4))/(H4*(L4-B4))))+((-I4*(L4-C4)*(-(J4*(M4-G4)-(J4*(L4-D4)*H4*(M4-E4))/(H4*(L4-B4)))/(I4*(M4-F4)-(I4*(L4-C4)*H4*(M4-E4))/(H4*(L4-B4))))-J4*(L4-D4))/(H4*(L4-B4)))+1)</f>
+        <v>1.6075486213000693E-2</v>
+      </c>
+      <c r="P4" s="1">
+        <f t="shared" si="1"/>
+        <v>0.91854531798340922</v>
+      </c>
+      <c r="Q4" s="1">
         <f t="shared" si="0"/>
-        <v>5.3565770875186908E-2</v>
-      </c>
-      <c r="L4" s="1">
-        <f t="shared" si="1"/>
-        <v>-6.0647922903512468</v>
-      </c>
-      <c r="M4" s="1">
-        <f t="shared" si="2"/>
-        <v>1.7442862950072215E-2</v>
-      </c>
-      <c r="N4" s="1">
-        <f t="shared" si="3"/>
-        <v>-0.31175772904281973</v>
-      </c>
-      <c r="O4" s="1">
-        <f t="shared" si="4"/>
-        <v>0.42402407781513007</v>
-      </c>
-      <c r="P4" s="1">
-        <f t="shared" si="5"/>
-        <v>8.7549258051186317E-3</v>
-      </c>
-      <c r="Q4" s="1">
-        <f t="shared" si="6"/>
-        <v>3.433940890149554E-2</v>
+        <v>0.1973549686158792</v>
       </c>
       <c r="R4" s="1">
-        <f t="shared" si="7"/>
-        <v>0.95690566529338583</v>
+        <f>(N4+O4)*K4*I4</f>
+        <v>138.17275005253217</v>
       </c>
       <c r="S4" s="1">
-        <f t="shared" si="8"/>
-        <v>0.79684276681094901</v>
+        <f>(H4*P4*B4 + I4*(N4+O4)*C4) / (H4*P4 + I4*(N4+O4))</f>
+        <v>0.84060110564725499</v>
       </c>
       <c r="T4" s="1">
-        <f t="shared" si="9"/>
-        <v>77.809106085472607</v>
-      </c>
-      <c r="U4" s="1">
-        <f t="shared" si="10"/>
-        <v>0.70415649701133265</v>
-      </c>
-      <c r="V4" s="1">
-        <f t="shared" si="11"/>
-        <v>5.9998515038535885E-2</v>
-      </c>
-      <c r="W4" s="1">
-        <f t="shared" si="12"/>
-        <v>0.33694787080495125</v>
+        <f>(H4*P4*E4 + I4*(N4+O4)*F4) / (H4*P4 + I4*(N4+O4))</f>
+        <v>6.9650939460586966E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>0.54450106867099102</v>
+        <v>0.52539567174907598</v>
       </c>
       <c r="C5" s="1">
-        <v>3.8788622521251299</v>
+        <v>3.9079031179597399</v>
       </c>
       <c r="D5" s="1">
-        <v>5.0697758493374399E-2</v>
+        <v>0.61207148136993506</v>
       </c>
       <c r="E5" s="1">
-        <v>0.25235308674579798</v>
+        <v>5.2478191314502598E-2</v>
       </c>
       <c r="F5" s="1">
-        <v>0.75030168566290201</v>
+        <v>0.24254286508707101</v>
       </c>
       <c r="G5" s="1">
-        <v>6.7124657057731199E-2</v>
+        <v>0.35166673573234902</v>
       </c>
       <c r="H5" s="1">
-        <v>1.3773272869450299</v>
+        <v>1.4207730031024799</v>
       </c>
       <c r="I5" s="1">
-        <v>1.7158991927288001</v>
+        <v>1.7525933265190199</v>
       </c>
       <c r="J5" s="1">
+        <v>1.49530361366891</v>
+      </c>
+      <c r="K5">
         <v>1000</v>
       </c>
-      <c r="K5" s="2">
+      <c r="L5" s="1">
+        <v>0.64399880687737399</v>
+      </c>
+      <c r="M5" s="1">
+        <v>7.1190445750567294E-2</v>
+      </c>
+      <c r="N5" s="1">
+        <f>(-(J5*(M5-G5)-(J5*(L5-D5)*H5*(M5-E5))/(H5*(L5-B5)))/(I5*(M5-F5)-(I5*(L5-C5)*H5*(M5-E5))/(H5*(L5-B5))))/((-(J5*(M5-G5)-(J5*(L5-D5)*H5*(M5-E5))/(H5*(L5-B5)))/(I5*(M5-F5)-(I5*(L5-C5)*H5*(M5-E5))/(H5*(L5-B5))))+((-I5*(L5-C5)*(-(J5*(M5-G5)-(J5*(L5-D5)*H5*(M5-E5))/(H5*(L5-B5)))/(I5*(M5-F5)-(I5*(L5-C5)*H5*(M5-E5))/(H5*(L5-B5))))-J5*(L5-D5))/(H5*(L5-B5)))+1)</f>
+        <v>2.7810527036894902E-2</v>
+      </c>
+      <c r="O5" s="1">
+        <f>1/((-(J5*(M5-G5)-(J5*(L5-D5)*H5*(M5-E5))/(H5*(L5-B5)))/(I5*(M5-F5)-(I5*(L5-C5)*H5*(M5-E5))/(H5*(L5-B5))))+((-I5*(L5-C5)*(-(J5*(M5-G5)-(J5*(L5-D5)*H5*(M5-E5))/(H5*(L5-B5)))/(I5*(M5-F5)-(I5*(L5-C5)*H5*(M5-E5))/(H5*(L5-B5))))-J5*(L5-D5))/(H5*(L5-B5)))+1)</f>
+        <v>3.9227248258126013E-2</v>
+      </c>
+      <c r="P5" s="1">
+        <f t="shared" si="1"/>
+        <v>0.93296222470497914</v>
+      </c>
+      <c r="Q5" s="1">
         <f t="shared" si="0"/>
-        <v>0.28345480545308199</v>
-      </c>
-      <c r="L5" s="1">
-        <f t="shared" si="1"/>
-        <v>-5.3682945503956949</v>
-      </c>
-      <c r="M5" s="1">
-        <f t="shared" si="2"/>
-        <v>2.2625215632566757E-2</v>
-      </c>
-      <c r="N5" s="1">
-        <f t="shared" si="3"/>
-        <v>-0.31783331297217715</v>
-      </c>
-      <c r="O5" s="1">
-        <f t="shared" si="4"/>
-        <v>0.43301245782973563</v>
-      </c>
-      <c r="P5" s="1">
-        <f t="shared" si="5"/>
-        <v>5.0153463574909879E-2</v>
-      </c>
-      <c r="Q5" s="1">
-        <f t="shared" si="6"/>
-        <v>1.2817278392492915E-2</v>
+        <v>0.58515140285449674</v>
       </c>
       <c r="R5" s="1">
-        <f t="shared" si="7"/>
-        <v>0.93702925803259718</v>
+        <f>(N5+O5)*K5*I5</f>
+        <v>117.48995760673529</v>
       </c>
       <c r="S5" s="1">
-        <f t="shared" si="8"/>
-        <v>0.20354339161396351</v>
+        <f>(H5*P5*B5 + I5*(N5+O5)*C5) / (H5*P5 + I5*(N5+O5))</f>
+        <v>0.8007981922520887</v>
       </c>
       <c r="T5" s="1">
-        <f t="shared" si="9"/>
-        <v>108.05144530740003</v>
-      </c>
-      <c r="U5" s="1">
-        <f t="shared" si="10"/>
-        <v>0.80209461383450287</v>
-      </c>
-      <c r="V5" s="1">
-        <f t="shared" si="11"/>
-        <v>6.6276487985373334E-2</v>
-      </c>
-      <c r="W5" s="1">
-        <f t="shared" si="12"/>
-        <v>0.36508378854885637</v>
+        <f>(H5*P5*E5 + I5*(N5+O5)*F5) / (H5*P5 + I5*(N5+O5))</f>
+        <v>6.7953187614714208E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>0.49262969520069499</v>
+        <v>0.49961508488867201</v>
       </c>
       <c r="C6" s="1">
-        <v>4.0110857996766898</v>
+        <v>3.82424379476931</v>
       </c>
       <c r="D6" s="1">
-        <v>5.1080733588183401E-2</v>
+        <v>0.59647310018732402</v>
       </c>
       <c r="E6" s="1">
-        <v>0.233627244997724</v>
+        <v>4.5365433708613102E-2</v>
       </c>
       <c r="F6" s="1">
-        <v>0.53713726974196796</v>
+        <v>0.23642688032998299</v>
       </c>
       <c r="G6" s="1">
-        <v>6.2730445581685404E-2</v>
+        <v>0.345709220188676</v>
       </c>
       <c r="H6" s="1">
-        <v>1.38675370330346</v>
+        <v>1.48724778165594</v>
       </c>
       <c r="I6" s="1">
-        <v>1.80111226346537</v>
+        <v>1.8893182938977799</v>
       </c>
       <c r="J6" s="1">
+        <v>1.6234338902821599</v>
+      </c>
+      <c r="K6">
         <v>1000</v>
       </c>
-      <c r="K6" s="2">
+      <c r="L6" s="1">
+        <v>0.71936769421051705</v>
+      </c>
+      <c r="M6" s="1">
+        <v>7.2751493605160006E-2</v>
+      </c>
+      <c r="N6" s="1">
+        <f>(-(J6*(M6-G6)-(J6*(L6-D6)*H6*(M6-E6))/(H6*(L6-B6)))/(I6*(M6-F6)-(I6*(L6-C6)*H6*(M6-E6))/(H6*(L6-B6))))/((-(J6*(M6-G6)-(J6*(L6-D6)*H6*(M6-E6))/(H6*(L6-B6)))/(I6*(M6-F6)-(I6*(L6-C6)*H6*(M6-E6))/(H6*(L6-B6))))+((-I6*(L6-C6)*(-(J6*(M6-G6)-(J6*(L6-D6)*H6*(M6-E6))/(H6*(L6-B6)))/(I6*(M6-F6)-(I6*(L6-C6)*H6*(M6-E6))/(H6*(L6-B6))))-J6*(L6-D6))/(H6*(L6-B6)))+1)</f>
+        <v>5.181408920040375E-2</v>
+      </c>
+      <c r="O6" s="1">
+        <f>1/((-(J6*(M6-G6)-(J6*(L6-D6)*H6*(M6-E6))/(H6*(L6-B6)))/(I6*(M6-F6)-(I6*(L6-C6)*H6*(M6-E6))/(H6*(L6-B6))))+((-I6*(L6-C6)*(-(J6*(M6-G6)-(J6*(L6-D6)*H6*(M6-E6))/(H6*(L6-B6)))/(I6*(M6-F6)-(I6*(L6-C6)*H6*(M6-E6))/(H6*(L6-B6))))-J6*(L6-D6))/(H6*(L6-B6)))+1)</f>
+        <v>4.670113914525869E-2</v>
+      </c>
+      <c r="P6" s="1">
+        <f t="shared" si="1"/>
+        <v>0.9014847716543376</v>
+      </c>
+      <c r="Q6" s="1">
         <f t="shared" si="0"/>
-        <v>6.1721043820165078E-2</v>
-      </c>
-      <c r="L6" s="1">
-        <f t="shared" si="1"/>
-        <v>-6.2569712999129221</v>
-      </c>
-      <c r="M6" s="1">
-        <f t="shared" si="2"/>
-        <v>1.6155281249407637E-2</v>
-      </c>
-      <c r="N6" s="1">
-        <f t="shared" si="3"/>
-        <v>-0.30780432121520857</v>
-      </c>
-      <c r="O6" s="1">
-        <f t="shared" si="4"/>
-        <v>0.42078889604502923</v>
-      </c>
-      <c r="P6" s="1">
-        <f t="shared" si="5"/>
-        <v>9.7680090218952246E-3</v>
-      </c>
-      <c r="Q6" s="1">
-        <f t="shared" si="6"/>
-        <v>3.0872584927748446E-2</v>
+        <v>0.47404995074870482</v>
       </c>
       <c r="R6" s="1">
-        <f t="shared" si="7"/>
-        <v>0.9593594060503563</v>
+        <f>(N6+O6)*K6*I6</f>
+        <v>186.12662314097716</v>
       </c>
       <c r="S6" s="1">
-        <f t="shared" si="8"/>
-        <v>0.75964896000293647</v>
+        <f>(H6*P6*B6 + I6*(N6+O6)*C6) / (H6*P6 + I6*(N6+O6))</f>
+        <v>0.90489309749182845</v>
       </c>
       <c r="T6" s="1">
-        <f t="shared" si="9"/>
-        <v>73.198272157219733</v>
-      </c>
-      <c r="U6" s="1">
-        <f t="shared" si="10"/>
-        <v>0.67611936720370236</v>
-      </c>
-      <c r="V6" s="1">
-        <f t="shared" si="11"/>
-        <v>6.0600647581488247E-2</v>
-      </c>
-      <c r="W6" s="1">
-        <f t="shared" si="12"/>
-        <v>0.3545152187766098</v>
+        <f>(H6*P6*E6 + I6*(N6+O6)*F6) / (H6*P6 + I6*(N6+O6))</f>
+        <v>6.8656155809900879E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>0.47813337886429402</v>
+        <v>0.483918729437257</v>
       </c>
       <c r="C7" s="1">
-        <v>4.5166821395389096</v>
+        <v>3.6047383884421298</v>
       </c>
       <c r="D7" s="1">
-        <v>5.2697259471646003E-2</v>
+        <v>0.57957357420065603</v>
       </c>
       <c r="E7" s="1">
-        <v>0.25811733365246098</v>
+        <v>4.9933367488007301E-2</v>
       </c>
       <c r="F7" s="1">
-        <v>0.52300615725110799</v>
+        <v>0.25673347582453898</v>
       </c>
       <c r="G7" s="1">
-        <v>6.11827323720191E-2</v>
+        <v>0.37124700690309298</v>
       </c>
       <c r="H7" s="1">
-        <v>1.3535452769785701</v>
+        <v>1.4061143094514801</v>
       </c>
       <c r="I7" s="1">
-        <v>1.7541933617085601</v>
+        <v>1.75981610794014</v>
       </c>
       <c r="J7" s="1">
+        <v>1.48224352449616</v>
+      </c>
+      <c r="K7">
         <v>1000</v>
       </c>
-      <c r="K7" s="2">
+      <c r="L7" s="1">
+        <v>0.79665728158674998</v>
+      </c>
+      <c r="M7" s="1">
+        <v>7.7103852911869303E-2</v>
+      </c>
+      <c r="N7" s="1">
+        <f>(-(J7*(M7-G7)-(J7*(L7-D7)*H7*(M7-E7))/(H7*(L7-B7)))/(I7*(M7-F7)-(I7*(L7-C7)*H7*(M7-E7))/(H7*(L7-B7))))/((-(J7*(M7-G7)-(J7*(L7-D7)*H7*(M7-E7))/(H7*(L7-B7)))/(I7*(M7-F7)-(I7*(L7-C7)*H7*(M7-E7))/(H7*(L7-B7))))+((-I7*(L7-C7)*(-(J7*(M7-G7)-(J7*(L7-D7)*H7*(M7-E7))/(H7*(L7-B7)))/(I7*(M7-F7)-(I7*(L7-C7)*H7*(M7-E7))/(H7*(L7-B7))))-J7*(L7-D7))/(H7*(L7-B7)))+1)</f>
+        <v>8.1280312619769604E-2</v>
+      </c>
+      <c r="O7" s="1">
+        <f>1/((-(J7*(M7-G7)-(J7*(L7-D7)*H7*(M7-E7))/(H7*(L7-B7)))/(I7*(M7-F7)-(I7*(L7-C7)*H7*(M7-E7))/(H7*(L7-B7))))+((-I7*(L7-C7)*(-(J7*(M7-G7)-(J7*(L7-D7)*H7*(M7-E7))/(H7*(L7-B7)))/(I7*(M7-F7)-(I7*(L7-C7)*H7*(M7-E7))/(H7*(L7-B7))))-J7*(L7-D7))/(H7*(L7-B7)))+1)</f>
+        <v>1.9834758923732401E-2</v>
+      </c>
+      <c r="P7" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89888492845649792</v>
+      </c>
+      <c r="Q7" s="1">
         <f t="shared" si="0"/>
-        <v>6.0737337250378109E-2</v>
-      </c>
-      <c r="L7" s="1">
-        <f t="shared" si="1"/>
-        <v>-7.0056798969441747</v>
-      </c>
-      <c r="M7" s="1">
-        <f t="shared" si="2"/>
-        <v>1.1485471767229654E-2</v>
-      </c>
-      <c r="N7" s="1">
-        <f t="shared" si="3"/>
-        <v>-0.34546137025687323</v>
-      </c>
-      <c r="O7" s="1">
-        <f t="shared" si="4"/>
-        <v>0.45278771323506056</v>
-      </c>
-      <c r="P7" s="1">
-        <f t="shared" si="5"/>
-        <v>8.5952096002014661E-3</v>
-      </c>
-      <c r="Q7" s="1">
-        <f t="shared" si="6"/>
-        <v>1.8590254545031465E-2</v>
+        <v>0.19616026197636655</v>
       </c>
       <c r="R7" s="1">
-        <f t="shared" si="7"/>
-        <v>0.97281453585476707</v>
+        <f>(N7+O7)*K7*I7</f>
+        <v>177.94393165777453</v>
       </c>
       <c r="S7" s="1">
-        <f t="shared" si="8"/>
-        <v>0.68383068413754977</v>
+        <f>(H7*P7*B7 + I7*(N7+O7)*C7) / (H7*P7 + I7*(N7+O7))</f>
+        <v>0.86906267124589875</v>
       </c>
       <c r="T7" s="1">
-        <f t="shared" si="9"/>
-        <v>47.688560738533674</v>
-      </c>
-      <c r="U7" s="1">
-        <f t="shared" si="10"/>
-        <v>0.6192850527185042</v>
-      </c>
-      <c r="V7" s="1">
-        <f t="shared" si="11"/>
-        <v>5.9876914598314464E-2</v>
-      </c>
-      <c r="W7" s="1">
-        <f t="shared" si="12"/>
-        <v>0.38721707268822986</v>
+        <f>(H7*P7*E7 + I7*(N7+O7)*F7) / (H7*P7 + I7*(N7+O7))</f>
+        <v>7.5454806594995941E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>0.48710610366756002</v>
+        <v>0.47870015822171103</v>
       </c>
       <c r="C8" s="1">
-        <v>4.1230972445694896</v>
+        <v>4.38871465518816</v>
       </c>
       <c r="D8" s="1">
-        <v>5.1780298003061602E-2</v>
+        <v>0.49847258343362399</v>
       </c>
       <c r="E8" s="1">
-        <v>0.240792773317617</v>
+        <v>4.7030522698803999E-2</v>
       </c>
       <c r="F8" s="1">
-        <v>0.54855895267588595</v>
+        <v>0.26888884033120303</v>
       </c>
       <c r="G8" s="1">
-        <v>6.3949076390641804E-2</v>
+        <v>0.39116172875563099</v>
       </c>
       <c r="H8" s="1">
-        <v>1.43901003589132</v>
+        <v>1.49513607861867</v>
       </c>
       <c r="I8" s="1">
-        <v>1.75969959036709</v>
+        <v>1.9135155676983699</v>
       </c>
       <c r="J8" s="1">
+        <v>1.5478557956335699</v>
+      </c>
+      <c r="K8">
         <v>1000</v>
       </c>
-      <c r="K8" s="2">
+      <c r="L8" s="1">
+        <v>0.58229403130966895</v>
+      </c>
+      <c r="M8" s="1">
+        <v>6.2409278423128003E-2</v>
+      </c>
+      <c r="N8" s="1">
+        <f>(-(J8*(M8-G8)-(J8*(L8-D8)*H8*(M8-E8))/(H8*(L8-B8)))/(I8*(M8-F8)-(I8*(L8-C8)*H8*(M8-E8))/(H8*(L8-B8))))/((-(J8*(M8-G8)-(J8*(L8-D8)*H8*(M8-E8))/(H8*(L8-B8)))/(I8*(M8-F8)-(I8*(L8-C8)*H8*(M8-E8))/(H8*(L8-B8))))+((-I8*(L8-C8)*(-(J8*(M8-G8)-(J8*(L8-D8)*H8*(M8-E8))/(H8*(L8-B8)))/(I8*(M8-F8)-(I8*(L8-C8)*H8*(M8-E8))/(H8*(L8-B8))))-J8*(L8-D8))/(H8*(L8-B8)))+1)</f>
+        <v>2.0731199097584113E-2</v>
+      </c>
+      <c r="O8" s="1">
+        <f>1/((-(J8*(M8-G8)-(J8*(L8-D8)*H8*(M8-E8))/(H8*(L8-B8)))/(I8*(M8-F8)-(I8*(L8-C8)*H8*(M8-E8))/(H8*(L8-B8))))+((-I8*(L8-C8)*(-(J8*(M8-G8)-(J8*(L8-D8)*H8*(M8-E8))/(H8*(L8-B8)))/(I8*(M8-F8)-(I8*(L8-C8)*H8*(M8-E8))/(H8*(L8-B8))))-J8*(L8-D8))/(H8*(L8-B8)))+1)</f>
+        <v>2.6935396909005954E-2</v>
+      </c>
+      <c r="P8" s="1">
+        <f t="shared" si="1"/>
+        <v>0.95233340399340993</v>
+      </c>
+      <c r="Q8" s="1">
         <f t="shared" si="0"/>
-        <v>8.8431266457094967E-2</v>
-      </c>
-      <c r="L8" s="1">
-        <f t="shared" si="1"/>
-        <v>-6.2901135679966513</v>
-      </c>
-      <c r="M8" s="1">
-        <f t="shared" si="2"/>
-        <v>1.7510994224265306E-2</v>
-      </c>
-      <c r="N8" s="1">
-        <f t="shared" si="3"/>
-        <v>-0.31119178104140011</v>
-      </c>
-      <c r="O8" s="1">
-        <f t="shared" si="4"/>
-        <v>0.42372294457036619</v>
-      </c>
-      <c r="P8" s="1">
-        <f t="shared" si="5"/>
-        <v>1.3863862174242781E-2</v>
-      </c>
-      <c r="Q8" s="1">
-        <f t="shared" si="6"/>
-        <v>3.0571637476053209E-2</v>
+        <v>0.56507909449380533</v>
       </c>
       <c r="R8" s="1">
-        <f t="shared" si="7"/>
-        <v>0.95556450034970408</v>
+        <f>(N8+O8)*K8*I8</f>
+        <v>91.210773517799055</v>
       </c>
       <c r="S8" s="1">
-        <f t="shared" si="8"/>
-        <v>0.688000308686741</v>
+        <f>(H8*P8*B8 + I8*(N8+O8)*C8) / (H8*P8 + I8*(N8+O8))</f>
+        <v>0.71409084920576615</v>
       </c>
       <c r="T8" s="1">
-        <f t="shared" si="9"/>
-        <v>78.193130532382824</v>
-      </c>
-      <c r="U8" s="1">
-        <f t="shared" si="10"/>
-        <v>0.68274179360529519</v>
-      </c>
-      <c r="V8" s="1">
-        <f t="shared" si="11"/>
-        <v>6.1950175921364141E-2</v>
-      </c>
-      <c r="W8" s="1">
-        <f t="shared" si="12"/>
-        <v>0.34623477295598509</v>
+        <f>(H8*P8*E8 + I8*(N8+O8)*F8) / (H8*P8 + I8*(N8+O8))</f>
+        <v>6.038683703691386E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>0.48187031873250402</v>
+        <v>0.48933604112020701</v>
       </c>
       <c r="C9" s="1">
-        <v>3.7994400531872299</v>
+        <v>3.86775867202685</v>
       </c>
       <c r="D9" s="1">
-        <v>4.8949623549682901E-2</v>
+        <v>0.54331256202881795</v>
       </c>
       <c r="E9" s="1">
-        <v>0.23866806333570301</v>
+        <v>5.0047673321102E-2</v>
       </c>
       <c r="F9" s="1">
-        <v>0.50226624022715605</v>
+        <v>0.25225390433679001</v>
       </c>
       <c r="G9" s="1">
-        <v>6.1370573191626802E-2</v>
+        <v>0.35502009883813301</v>
       </c>
       <c r="H9" s="1">
-        <v>1.44382225999346</v>
+        <v>1.5589376527113801</v>
       </c>
       <c r="I9" s="1">
-        <v>1.7633845750139501</v>
+        <v>1.88473989501647</v>
       </c>
       <c r="J9" s="1">
+        <v>1.6185190890229499</v>
+      </c>
+      <c r="K9">
         <v>1000</v>
       </c>
-      <c r="K9" s="2">
+      <c r="L9" s="1">
+        <v>0.543715904601907</v>
+      </c>
+      <c r="M9" s="1">
+        <v>5.8993050858270203E-2</v>
+      </c>
+      <c r="N9" s="1">
+        <f>(-(J9*(M9-G9)-(J9*(L9-D9)*H9*(M9-E9))/(H9*(L9-B9)))/(I9*(M9-F9)-(I9*(L9-C9)*H9*(M9-E9))/(H9*(L9-B9))))/((-(J9*(M9-G9)-(J9*(L9-D9)*H9*(M9-E9))/(H9*(L9-B9)))/(I9*(M9-F9)-(I9*(L9-C9)*H9*(M9-E9))/(H9*(L9-B9))))+((-I9*(L9-C9)*(-(J9*(M9-G9)-(J9*(L9-D9)*H9*(M9-E9))/(H9*(L9-B9)))/(I9*(M9-F9)-(I9*(L9-C9)*H9*(M9-E9))/(H9*(L9-B9))))-J9*(L9-D9))/(H9*(L9-B9)))+1)</f>
+        <v>1.3109451907197842E-2</v>
+      </c>
+      <c r="O9" s="1">
+        <f>1/((-(J9*(M9-G9)-(J9*(L9-D9)*H9*(M9-E9))/(H9*(L9-B9)))/(I9*(M9-F9)-(I9*(L9-C9)*H9*(M9-E9))/(H9*(L9-B9))))+((-I9*(L9-C9)*(-(J9*(M9-G9)-(J9*(L9-D9)*H9*(M9-E9))/(H9*(L9-B9)))/(I9*(M9-F9)-(I9*(L9-C9)*H9*(M9-E9))/(H9*(L9-B9))))-J9*(L9-D9))/(H9*(L9-B9)))+1)</f>
+        <v>1.8227405028062412E-2</v>
+      </c>
+      <c r="P9" s="1">
+        <f t="shared" si="1"/>
+        <v>0.96866314306473977</v>
+      </c>
+      <c r="Q9" s="1">
         <f t="shared" si="0"/>
-        <v>2.9448085467057676E-2</v>
-      </c>
-      <c r="L9" s="1">
-        <f t="shared" si="1"/>
-        <v>-5.8141854429137254</v>
-      </c>
-      <c r="M9" s="1">
-        <f t="shared" si="2"/>
-        <v>1.7933643583296403E-2</v>
-      </c>
-      <c r="N9" s="1">
-        <f t="shared" si="3"/>
-        <v>-0.31264365930875182</v>
-      </c>
-      <c r="O9" s="1">
-        <f t="shared" si="4"/>
-        <v>0.42086358143463115</v>
-      </c>
-      <c r="P9" s="1">
-        <f t="shared" si="5"/>
-        <v>5.039345010948602E-3</v>
-      </c>
-      <c r="Q9" s="1">
-        <f t="shared" si="6"/>
-        <v>3.8653262526972133E-2</v>
+        <v>0.58166028155660121</v>
       </c>
       <c r="R9" s="1">
-        <f t="shared" si="7"/>
-        <v>0.9563073924620793</v>
+        <f>(N9+O9)*K9*I9</f>
+        <v>59.061824450308549</v>
       </c>
       <c r="S9" s="1">
-        <f t="shared" si="8"/>
-        <v>0.88466366978498678</v>
+        <f>(H9*P9*B9 + I9*(N9+O9)*C9) / (H9*P9 + I9*(N9+O9))</f>
+        <v>0.61649797680168417</v>
       </c>
       <c r="T9" s="1">
-        <f t="shared" si="9"/>
-        <v>77.046870174507674</v>
-      </c>
-      <c r="U9" s="1">
-        <f t="shared" si="10"/>
-        <v>0.65721058139954469</v>
-      </c>
-      <c r="V9" s="1">
-        <f t="shared" si="11"/>
-        <v>5.8976626364238463E-2</v>
-      </c>
-      <c r="W9" s="1">
-        <f t="shared" si="12"/>
-        <v>0.34044227683273831</v>
+        <f>(H9*P9*E9 + I9*(N9+O9)*F9) / (H9*P9 + I9*(N9+O9))</f>
+        <v>5.7658602607326463E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>0.50092466747574205</v>
+        <v>0.504658580641968</v>
       </c>
       <c r="C10" s="1">
-        <v>4.0359712561079997</v>
+        <v>3.8240843321571898</v>
       </c>
       <c r="D10" s="1">
-        <v>5.2858006151306598E-2</v>
+        <v>0.57574458607115897</v>
       </c>
       <c r="E10" s="1">
-        <v>0.24014344879670799</v>
+        <v>4.9421254902723498E-2</v>
       </c>
       <c r="F10" s="1">
-        <v>0.53698000201130502</v>
+        <v>0.225879289160928</v>
       </c>
       <c r="G10" s="1">
-        <v>6.1526083700679697E-2</v>
+        <v>0.336990822035239</v>
       </c>
       <c r="H10" s="1">
-        <v>1.3745484884947601</v>
+        <v>1.3385227295297</v>
       </c>
       <c r="I10" s="1">
-        <v>1.8026290929342601</v>
+        <v>1.70408895546707</v>
       </c>
       <c r="J10" s="1">
+        <v>1.35770514630642</v>
+      </c>
+      <c r="K10">
         <v>1000</v>
       </c>
-      <c r="K10" s="2">
+      <c r="L10" s="1">
+        <v>0.58168222005873504</v>
+      </c>
+      <c r="M10" s="1">
+        <v>6.1062091898683502E-2</v>
+      </c>
+      <c r="N10" s="1">
+        <f>(-(J10*(M10-G10)-(J10*(L10-D10)*H10*(M10-E10))/(H10*(L10-B10)))/(I10*(M10-F10)-(I10*(L10-C10)*H10*(M10-E10))/(H10*(L10-B10))))/((-(J10*(M10-G10)-(J10*(L10-D10)*H10*(M10-E10))/(H10*(L10-B10)))/(I10*(M10-F10)-(I10*(L10-C10)*H10*(M10-E10))/(H10*(L10-B10))))+((-I10*(L10-C10)*(-(J10*(M10-G10)-(J10*(L10-D10)*H10*(M10-E10))/(H10*(L10-B10)))/(I10*(M10-F10)-(I10*(L10-C10)*H10*(M10-E10))/(H10*(L10-B10))))-J10*(L10-D10))/(H10*(L10-B10)))+1)</f>
+        <v>1.7872337213226331E-2</v>
+      </c>
+      <c r="O10" s="1">
+        <f>1/((-(J10*(M10-G10)-(J10*(L10-D10)*H10*(M10-E10))/(H10*(L10-B10)))/(I10*(M10-F10)-(I10*(L10-C10)*H10*(M10-E10))/(H10*(L10-B10))))+((-I10*(L10-C10)*(-(J10*(M10-G10)-(J10*(L10-D10)*H10*(M10-E10))/(H10*(L10-B10)))/(I10*(M10-F10)-(I10*(L10-C10)*H10*(M10-E10))/(H10*(L10-B10))))-J10*(L10-D10))/(H10*(L10-B10)))+1)</f>
+        <v>2.6353320062274591E-2</v>
+      </c>
+      <c r="P10" s="1">
+        <f t="shared" si="1"/>
+        <v>0.95577434272449902</v>
+      </c>
+      <c r="Q10" s="1">
         <f t="shared" si="0"/>
-        <v>4.9559805588031011E-2</v>
-      </c>
-      <c r="L10" s="1">
-        <f t="shared" si="1"/>
-        <v>-6.307383430557234</v>
-      </c>
-      <c r="M10" s="1">
-        <f t="shared" si="2"/>
-        <v>1.1914692893646156E-2</v>
-      </c>
-      <c r="N10" s="1">
-        <f t="shared" si="3"/>
-        <v>-0.32198085882536104</v>
-      </c>
-      <c r="O10" s="1">
-        <f t="shared" si="4"/>
-        <v>0.43288956727851463</v>
-      </c>
-      <c r="P10" s="1">
-        <f t="shared" si="5"/>
-        <v>7.7961692824684049E-3</v>
-      </c>
-      <c r="Q10" s="1">
-        <f t="shared" si="6"/>
-        <v>2.151030506076081E-2</v>
+        <v>0.59588306168313698</v>
       </c>
       <c r="R10" s="1">
-        <f t="shared" si="7"/>
-        <v>0.97069352565677081</v>
+        <f>(N10+O10)*K10*I10</f>
+        <v>75.364454111452986</v>
       </c>
       <c r="S10" s="1">
-        <f t="shared" si="8"/>
-        <v>0.73397791931018874</v>
+        <f>(H10*P10*B10 + I10*(N10+O10)*C10) / (H10*P10 + I10*(N10+O10))</f>
+        <v>0.6893256886770972</v>
       </c>
       <c r="T10" s="1">
-        <f t="shared" si="9"/>
-        <v>52.828703262436449</v>
-      </c>
-      <c r="U10" s="1">
-        <f t="shared" si="10"/>
-        <v>0.63556004497864726</v>
-      </c>
-      <c r="V10" s="1">
-        <f t="shared" si="11"/>
-        <v>5.9990937963986989E-2</v>
-      </c>
-      <c r="W10" s="1">
-        <f t="shared" si="12"/>
-        <v>0.36779019726852441</v>
+        <f>(H10*P10*E10 + I10*(N10+O10)*F10) / (H10*P10 + I10*(N10+O10))</f>
+        <v>5.9238011569490885E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>0.482710794744099</v>
+        <v>0.53719843112493004</v>
       </c>
       <c r="C11" s="1">
-        <v>4.1861839630687596</v>
+        <v>3.9826023506793802</v>
       </c>
       <c r="D11" s="1">
-        <v>4.7781427736663599E-2</v>
+        <v>0.61182359145490095</v>
       </c>
       <c r="E11" s="1">
-        <v>0.261462004061224</v>
+        <v>5.3020223060988601E-2</v>
       </c>
       <c r="F11" s="1">
-        <v>0.59844067583265703</v>
+        <v>0.229371400969753</v>
       </c>
       <c r="G11" s="1">
-        <v>5.7003357441402301E-2</v>
+        <v>0.35076447662277399</v>
       </c>
       <c r="H11" s="1">
-        <v>1.4000417868231601</v>
+        <v>1.4518256868383701</v>
       </c>
       <c r="I11" s="1">
-        <v>1.8293307627692199</v>
+        <v>1.8845974415377</v>
       </c>
       <c r="J11" s="1">
+        <v>1.5875354202290799</v>
+      </c>
+      <c r="K11">
         <v>1000</v>
       </c>
-      <c r="K11" s="2">
+      <c r="L11" s="1">
+        <v>0.56716997836734095</v>
+      </c>
+      <c r="M11" s="1">
+        <v>6.6938954848764595E-2</v>
+      </c>
+      <c r="N11" s="1">
+        <f>(-(J11*(M11-G11)-(J11*(L11-D11)*H11*(M11-E11))/(H11*(L11-B11)))/(I11*(M11-F11)-(I11*(L11-C11)*H11*(M11-E11))/(H11*(L11-B11))))/((-(J11*(M11-G11)-(J11*(L11-D11)*H11*(M11-E11))/(H11*(L11-B11)))/(I11*(M11-F11)-(I11*(L11-C11)*H11*(M11-E11))/(H11*(L11-B11))))+((-I11*(L11-C11)*(-(J11*(M11-G11)-(J11*(L11-D11)*H11*(M11-E11))/(H11*(L11-B11)))/(I11*(M11-F11)-(I11*(L11-C11)*H11*(M11-E11))/(H11*(L11-B11))))-J11*(L11-D11))/(H11*(L11-B11)))+1)</f>
+        <v>6.0308416743351965E-3</v>
+      </c>
+      <c r="O11" s="1">
+        <f>1/((-(J11*(M11-G11)-(J11*(L11-D11)*H11*(M11-E11))/(H11*(L11-B11)))/(I11*(M11-F11)-(I11*(L11-C11)*H11*(M11-E11))/(H11*(L11-B11))))+((-I11*(L11-C11)*(-(J11*(M11-G11)-(J11*(L11-D11)*H11*(M11-E11))/(H11*(L11-B11)))/(I11*(M11-F11)-(I11*(L11-C11)*H11*(M11-E11))/(H11*(L11-B11))))-J11*(L11-D11))/(H11*(L11-B11)))+1)</f>
+        <v>3.8742366960811077E-2</v>
+      </c>
+      <c r="P11" s="1">
+        <f t="shared" si="1"/>
+        <v>0.95522679136485367</v>
+      </c>
+      <c r="Q11" s="1">
         <f t="shared" si="0"/>
-        <v>0.16202666950805661</v>
-      </c>
-      <c r="L11" s="1">
-        <f t="shared" si="1"/>
-        <v>-6.5631691642597678</v>
-      </c>
-      <c r="M11" s="1">
-        <f t="shared" si="2"/>
-        <v>1.2911086941779948E-2</v>
-      </c>
-      <c r="N11" s="1">
-        <f t="shared" si="3"/>
-        <v>-0.37402249197580079</v>
-      </c>
-      <c r="O11" s="1">
-        <f t="shared" si="4"/>
-        <v>0.47830048732448777</v>
-      </c>
-      <c r="P11" s="1">
-        <f t="shared" si="5"/>
-        <v>2.4092483477507948E-2</v>
-      </c>
-      <c r="Q11" s="1">
-        <f t="shared" si="6"/>
-        <v>7.5034338871169549E-3</v>
+        <v>0.86530244630265174</v>
       </c>
       <c r="R11" s="1">
-        <f t="shared" si="7"/>
-        <v>0.96840408263537514</v>
+        <f>(N11+O11)*K11*I11</f>
+        <v>84.379474443230322</v>
       </c>
       <c r="S11" s="1">
-        <f t="shared" si="8"/>
-        <v>0.2374811213906349</v>
+        <f>(H11*P11*B11 + I11*(N11+O11)*C11) / (H11*P11 + I11*(N11+O11))</f>
+        <v>0.73480645451974036</v>
       </c>
       <c r="T11" s="1">
-        <f t="shared" si="9"/>
-        <v>57.799383613022506</v>
-      </c>
-      <c r="U11" s="1">
-        <f t="shared" si="10"/>
-        <v>0.6341380892669809</v>
-      </c>
-      <c r="V11" s="1">
-        <f t="shared" si="11"/>
-        <v>5.6518380886929231E-2</v>
-      </c>
-      <c r="W11" s="1">
-        <f t="shared" si="12"/>
-        <v>0.38941443599836784</v>
+        <f>(H11*P11*E11 + I11*(N11+O11)*F11) / (H11*P11 + I11*(N11+O11))</f>
+        <v>6.3134685255715528E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>